<commit_message>
Add partnumber in search bar
</commit_message>
<xml_diff>
--- a/begbal_format.xlsx
+++ b/begbal_format.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="144">
   <si>
     <t>Item ID</t>
   </si>
@@ -41,7 +41,7 @@
     <t>begbal</t>
   </si>
   <si>
-    <t>2022-08-30</t>
+    <t>2022-09-24</t>
   </si>
   <si>
     <t>Just fill out quantity column. Do not edit other columns.</t>
@@ -84,6 +84,372 @@
   </si>
   <si>
     <t>Cover</t>
+  </si>
+  <si>
+    <t>Thrust Ball Bearing</t>
+  </si>
+  <si>
+    <t>Oring, 700 x 6mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slotted Set Screw
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gasket, 1 mm thick</t>
+  </si>
+  <si>
+    <t>O-ring</t>
+  </si>
+  <si>
+    <t>O-ring, 59.69 mm x 5.33 mm</t>
+  </si>
+  <si>
+    <t>O-ring - Brand New</t>
+  </si>
+  <si>
+    <t>O-ring, 26 mm x 7 mm - Brand New</t>
+  </si>
+  <si>
+    <t>Bolt, Allen, Half Thread, M18 x 50mm x 2.5 Pitch</t>
+  </si>
+  <si>
+    <t>Oring, 290 x 5mm</t>
+  </si>
+  <si>
+    <t>Gate Valve, 2", used</t>
+  </si>
+  <si>
+    <t>Return Pipe Bellows (sm)</t>
+  </si>
+  <si>
+    <t>O-ring, 3mm x 56mm</t>
+  </si>
+  <si>
+    <t>Packing - Brand New for Inspection Door for Crank Case</t>
+  </si>
+  <si>
+    <t>Packing / Gasket, 1.5MM</t>
+  </si>
+  <si>
+    <t>O-ring for Cylinder</t>
+  </si>
+  <si>
+    <t>Packing/Gasket, PN 02125006978 / 25125002400 - Brand New</t>
+  </si>
+  <si>
+    <t>Control Rack</t>
+  </si>
+  <si>
+    <t>Lower Spring Collar - Reconditioned</t>
+  </si>
+  <si>
+    <t>Guide for Plunger</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 
+Packing/Gasket/Joint</t>
+  </si>
+  <si>
+    <t>O-ring for Fuel Injector</t>
+  </si>
+  <si>
+    <t>O-ring (Old)</t>
+  </si>
+  <si>
+    <t>O-ring for Fuel Injection Pipe</t>
+  </si>
+  <si>
+    <t>Exhuast Valve</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 
+Roller Bush</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Roller</t>
+  </si>
+  <si>
+    <t>Fitted Bolt / Reamer Bolt PF 71-14</t>
+  </si>
+  <si>
+    <t>Nut, M12</t>
+  </si>
+  <si>
+    <t>Washer M13</t>
+  </si>
+  <si>
+    <t>Split Pin</t>
+  </si>
+  <si>
+    <t>Torque Wrench, changeable head, 110.6-590ft/lbs 150-180NM, dual pin shank Adjustable, Model: 800NMIMH</t>
+  </si>
+  <si>
+    <t>Open End Head, CDI 65mm, "Z" shank dual pin, TCQZOM65ADP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open End Head, CDI 55mm, "Z" shank dual pin, TCQZOM55ADP        </t>
+  </si>
+  <si>
+    <t>Open End Head, CDI 41mm, "Z" shank dual pin, TCQZOM41ADP</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hose Clip 4", No. 56</t>
+  </si>
+  <si>
+    <t>Copper Packing, 38 mm x 30.5 mm x 2 mmT</t>
+  </si>
+  <si>
+    <t>Rectifier, Reverse, 1400V, 150A, DO-8</t>
+  </si>
+  <si>
+    <t>Rectifier, Forward, 1400V, 150A, DO-8</t>
+  </si>
+  <si>
+    <t>Injector Nozzle, 10 holes x 0.65 R x 140 deg</t>
+  </si>
+  <si>
+    <t>Copper Ring</t>
+  </si>
+  <si>
+    <t>Ball Bearing, SKF 6202-2Z/C3</t>
+  </si>
+  <si>
+    <t>Bulb, Pilot, 120V</t>
+  </si>
+  <si>
+    <t>Ball Bearing, SKF 6208-2Z/C3</t>
+  </si>
+  <si>
+    <t>Push Rod</t>
+  </si>
+  <si>
+    <t>Indicator Valve Assembly</t>
+  </si>
+  <si>
+    <t>Bellows</t>
+  </si>
+  <si>
+    <t>Bolt, Hex, Full Thread, Grade 8.8, M12 x 50mm x 1.75 Pitch</t>
+  </si>
+  <si>
+    <t>Bolt, Hex, Half Thread, SS, M12 x 48mm x 1.75 Pitch</t>
+  </si>
+  <si>
+    <t>Mechanical Seal, 55mm</t>
+  </si>
+  <si>
+    <t>Spindle, Complete - Reconditioned</t>
+  </si>
+  <si>
+    <t>Hose Clip, No.40, 3"- 1-1/2 , 76-38mm</t>
+  </si>
+  <si>
+    <t>Top Ring, PF 5-20</t>
+  </si>
+  <si>
+    <t>Compression Ring, PF 5-21</t>
+  </si>
+  <si>
+    <t>Compression Ring, PF 5-23</t>
+  </si>
+  <si>
+    <t>Oil Scrapper, PF 5-22</t>
+  </si>
+  <si>
+    <t>Packing/Gasket</t>
+  </si>
+  <si>
+    <t>Piston Seal Ring, Set, 190 x 184 x 5.8, 170.82 x 5.33mm, PN 9410.01, POS 4+4A</t>
+  </si>
+  <si>
+    <t>Rod Seal Ring, Set, 110 x 115 x 3.8, 113.9 x 3.53mm, PN 9410.01, POS. 5+5A</t>
+  </si>
+  <si>
+    <t>Piston Seal Ring, Set, 120 x 115 x 3.8, 107.55 x 3.53, PN 9427.01, POS. 4+4A</t>
+  </si>
+  <si>
+    <t>Rod Seal Ring, Set, 75 x 79 x 3.8, 78.97 x 3.53mm, PN 9427.01, POS. 5+5A</t>
+  </si>
+  <si>
+    <t>Piston Seal Ring, Set, 190 x 184 x 5.8, 170.82 x 5.33mm, PN 9419.01, POS. 4+4A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rod Seal Ring, Set, 130 x 135 x 3.8, 113.9 x 3.53mm, PN 9419.01, POS. 5+5A   </t>
+  </si>
+  <si>
+    <t>Piston Seal Ring, Set, 120 x 115 x 3.8, 107.55 x 3.53mm, PN 9433.07, POS. 4+4A</t>
+  </si>
+  <si>
+    <t>Rod Seal Ring, Set, 60 x 64 x 3.8, 63.10 x 3.53mm, PN 9433.07, POS. 5+5A</t>
+  </si>
+  <si>
+    <t>Cylinder Head Assembly (Complete)</t>
+  </si>
+  <si>
+    <t>Cylinder Liner with Water Jacket - Reconditioned</t>
+  </si>
+  <si>
+    <t>Piston, Complete - Reconditioned</t>
+  </si>
+  <si>
+    <t>Connecting Rod, Complete - Reconditioned</t>
+  </si>
+  <si>
+    <t>Upper Guide Bush, Inlet/Exhaust Valves, 30mm x 60mm, Tapered</t>
+  </si>
+  <si>
+    <t>O - ring</t>
+  </si>
+  <si>
+    <t>O-ring, 2.5mm x 70mm</t>
+  </si>
+  <si>
+    <t>Lower Guide Bush, Inlet/Exhaust Valves, 30mm x 70mm, Carbon Steel</t>
+  </si>
+  <si>
+    <t>O-ring, 5mm x 124mm - Brand New</t>
+  </si>
+  <si>
+    <t>Bolt, Hex, Full Thread, Grade 8.8, M10 x 30mm x 1.5 Pitch</t>
+  </si>
+  <si>
+    <t>Bolt, Hex, Full Thread, M20 x 50mm x 2.5 Pitch</t>
+  </si>
+  <si>
+    <t>Packing / Special Joint, PF 16-6</t>
+  </si>
+  <si>
+    <t>Tube Finned, 36", IRHP-11/19</t>
+  </si>
+  <si>
+    <t>Delivery Valve Spring, PF 30-9</t>
+  </si>
+  <si>
+    <t>Delivery Valve, PF 30-8</t>
+  </si>
+  <si>
+    <t>Inner Spring</t>
+  </si>
+  <si>
+    <t>Connecting Rod</t>
+  </si>
+  <si>
+    <t>Spring Collar</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>Spring Guide - Reconditioned</t>
+  </si>
+  <si>
+    <t>Nut (Lock), PF 102-87</t>
+  </si>
+  <si>
+    <t>Connection Pipe - Reconditioned</t>
+  </si>
+  <si>
+    <t>O-ring for Starting Valve</t>
+  </si>
+  <si>
+    <t>Bolt, Hex, Half Thread, Grade 8.8, M12 x 55mm x 1.75 Pitch</t>
+  </si>
+  <si>
+    <t>Bolt, Stud, Full Thread, M18 x 92mm x 2.5 Pitch</t>
+  </si>
+  <si>
+    <t>Nut, M19</t>
+  </si>
+  <si>
+    <t>Self Lock Nut, PF 10-35</t>
+  </si>
+  <si>
+    <t>Bolt, Stud, HT, M12 x 65mm w/ nut</t>
+  </si>
+  <si>
+    <t>Upper Guide Bush, Inlet/Exhaust Valves, 30mm x 60mm, Carbon Steel</t>
+  </si>
+  <si>
+    <t>Control Pinion</t>
+  </si>
+  <si>
+    <t>O-ring, 40.64 mm x 3.53 mm</t>
+  </si>
+  <si>
+    <t>Ball Bearing, 6313, SJ8-V19</t>
+  </si>
+  <si>
+    <t>Fuel Cam (upper)</t>
+  </si>
+  <si>
+    <t>Fuel Cam (lower)</t>
+  </si>
+  <si>
+    <t>O-ring, 3mm x 41mm</t>
+  </si>
+  <si>
+    <t>O-ring, 3mm x 50mm</t>
+  </si>
+  <si>
+    <t>Hexagonal Socket Screw Head, PF 30-7, 14mm OD x 82mm L</t>
+  </si>
+  <si>
+    <t>Protecting Pipe - Reconditioned</t>
+  </si>
+  <si>
+    <t>Tie Rod</t>
+  </si>
+  <si>
+    <t>Cylinder Head Nut, PF 8-4</t>
+  </si>
+  <si>
+    <t>Gasket, Copper, 0.5x20mm</t>
+  </si>
+  <si>
+    <t>Delivery Valve Piece</t>
+  </si>
+  <si>
+    <t>Fuel Injection Pipe</t>
+  </si>
+  <si>
+    <t>Bulb, Pilot, 130V, 2.6W</t>
+  </si>
+  <si>
+    <t>Fuel Injection Pump Complete - Reconditioned with new plunger and barrel</t>
+  </si>
+  <si>
+    <t>Thyristor / Diode Modules, SKKH 106/08 E, SEMIPACK</t>
+  </si>
+  <si>
+    <t>Injection Pump Operating Gear</t>
+  </si>
+  <si>
+    <t>Washer for Fuel Pump Drive</t>
+  </si>
+  <si>
+    <t>Cable, Royal Cord, 3.5mm² x 3C</t>
+  </si>
+  <si>
+    <t>Magnetic Wire, ES-GP200-AWG-HVY-NAT</t>
+  </si>
+  <si>
+    <t>Plunger and Barrel - Brand New</t>
+  </si>
+  <si>
+    <t>Barrel- Refurbished</t>
+  </si>
+  <si>
+    <t>Plunger- Refurbished</t>
+  </si>
+  <si>
+    <t>Connector</t>
+  </si>
+  <si>
+    <t>Oring, 375 x 6mm</t>
+  </si>
+  <si>
+    <t>Oring, 170 x 5mm</t>
   </si>
 </sst>
 </file>
@@ -434,7 +800,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I143"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="I1" sqref="I1"/>
@@ -672,6 +1038,1926 @@
       </c>
       <c r="D15"/>
       <c r="E15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16"/>
+      <c r="E16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17"/>
+      <c r="E17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18"/>
+      <c r="E18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19"/>
+      <c r="E19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20"/>
+      <c r="E20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21"/>
+      <c r="E21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22"/>
+      <c r="E22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23"/>
+      <c r="E23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24"/>
+      <c r="E24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25"/>
+      <c r="E25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26"/>
+      <c r="E26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27"/>
+      <c r="E27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28"/>
+      <c r="E28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29"/>
+      <c r="E29" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30"/>
+      <c r="E30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31"/>
+      <c r="E31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32"/>
+      <c r="E32" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33"/>
+      <c r="E33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34"/>
+      <c r="E34" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35"/>
+      <c r="E35" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36"/>
+      <c r="E36" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>42</v>
+      </c>
+      <c r="C37" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37"/>
+      <c r="E37" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>27</v>
+      </c>
+      <c r="C38" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38"/>
+      <c r="E38" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>22</v>
+      </c>
+      <c r="C39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39"/>
+      <c r="E39" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>43</v>
+      </c>
+      <c r="C40" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40"/>
+      <c r="E40" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>44</v>
+      </c>
+      <c r="C41" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41"/>
+      <c r="E41" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>45</v>
+      </c>
+      <c r="C42" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42"/>
+      <c r="E42" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>46</v>
+      </c>
+      <c r="C43" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43"/>
+      <c r="E43" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>47</v>
+      </c>
+      <c r="C44" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44"/>
+      <c r="E44" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>48</v>
+      </c>
+      <c r="C45" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45"/>
+      <c r="E45" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>49</v>
+      </c>
+      <c r="C46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46"/>
+      <c r="E46" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>50</v>
+      </c>
+      <c r="C47" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47"/>
+      <c r="E47" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>51</v>
+      </c>
+      <c r="C48" t="s">
+        <v>7</v>
+      </c>
+      <c r="D48"/>
+      <c r="E48" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>52</v>
+      </c>
+      <c r="C49" t="s">
+        <v>7</v>
+      </c>
+      <c r="D49"/>
+      <c r="E49" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>53</v>
+      </c>
+      <c r="C50" t="s">
+        <v>7</v>
+      </c>
+      <c r="D50"/>
+      <c r="E50" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>54</v>
+      </c>
+      <c r="C51" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51"/>
+      <c r="E51" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52"/>
+      <c r="E52" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>56</v>
+      </c>
+      <c r="C53" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53"/>
+      <c r="E53" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C54" t="s">
+        <v>7</v>
+      </c>
+      <c r="D54"/>
+      <c r="E54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>58</v>
+      </c>
+      <c r="C55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D55"/>
+      <c r="E55" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>59</v>
+      </c>
+      <c r="C56" t="s">
+        <v>7</v>
+      </c>
+      <c r="D56"/>
+      <c r="E56" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>60</v>
+      </c>
+      <c r="C57" t="s">
+        <v>7</v>
+      </c>
+      <c r="D57"/>
+      <c r="E57" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>61</v>
+      </c>
+      <c r="C58" t="s">
+        <v>7</v>
+      </c>
+      <c r="D58"/>
+      <c r="E58" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>62</v>
+      </c>
+      <c r="C59" t="s">
+        <v>7</v>
+      </c>
+      <c r="D59"/>
+      <c r="E59" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>63</v>
+      </c>
+      <c r="C60" t="s">
+        <v>7</v>
+      </c>
+      <c r="D60"/>
+      <c r="E60" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>64</v>
+      </c>
+      <c r="C61" t="s">
+        <v>7</v>
+      </c>
+      <c r="D61"/>
+      <c r="E61" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>65</v>
+      </c>
+      <c r="C62" t="s">
+        <v>7</v>
+      </c>
+      <c r="D62"/>
+      <c r="E62" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>66</v>
+      </c>
+      <c r="C63" t="s">
+        <v>7</v>
+      </c>
+      <c r="D63"/>
+      <c r="E63" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>67</v>
+      </c>
+      <c r="C64" t="s">
+        <v>7</v>
+      </c>
+      <c r="D64"/>
+      <c r="E64" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>68</v>
+      </c>
+      <c r="C65" t="s">
+        <v>7</v>
+      </c>
+      <c r="D65"/>
+      <c r="E65" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>69</v>
+      </c>
+      <c r="C66" t="s">
+        <v>7</v>
+      </c>
+      <c r="D66"/>
+      <c r="E66" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>70</v>
+      </c>
+      <c r="C67" t="s">
+        <v>7</v>
+      </c>
+      <c r="D67"/>
+      <c r="E67" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>71</v>
+      </c>
+      <c r="C68" t="s">
+        <v>7</v>
+      </c>
+      <c r="D68"/>
+      <c r="E68" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>72</v>
+      </c>
+      <c r="C69" t="s">
+        <v>7</v>
+      </c>
+      <c r="D69"/>
+      <c r="E69" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>73</v>
+      </c>
+      <c r="C70" t="s">
+        <v>7</v>
+      </c>
+      <c r="D70"/>
+      <c r="E70" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>74</v>
+      </c>
+      <c r="C71" t="s">
+        <v>7</v>
+      </c>
+      <c r="D71"/>
+      <c r="E71" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>75</v>
+      </c>
+      <c r="C72" t="s">
+        <v>7</v>
+      </c>
+      <c r="D72"/>
+      <c r="E72" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>76</v>
+      </c>
+      <c r="C73" t="s">
+        <v>7</v>
+      </c>
+      <c r="D73"/>
+      <c r="E73" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
+        <v>77</v>
+      </c>
+      <c r="C74" t="s">
+        <v>7</v>
+      </c>
+      <c r="D74"/>
+      <c r="E74" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>78</v>
+      </c>
+      <c r="C75" t="s">
+        <v>7</v>
+      </c>
+      <c r="D75"/>
+      <c r="E75" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>79</v>
+      </c>
+      <c r="C76" t="s">
+        <v>7</v>
+      </c>
+      <c r="D76"/>
+      <c r="E76" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
+        <v>80</v>
+      </c>
+      <c r="C77" t="s">
+        <v>7</v>
+      </c>
+      <c r="D77"/>
+      <c r="E77" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
+        <v>81</v>
+      </c>
+      <c r="C78" t="s">
+        <v>7</v>
+      </c>
+      <c r="D78"/>
+      <c r="E78" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
+        <v>82</v>
+      </c>
+      <c r="C79" t="s">
+        <v>7</v>
+      </c>
+      <c r="D79"/>
+      <c r="E79" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
+        <v>83</v>
+      </c>
+      <c r="C80" t="s">
+        <v>7</v>
+      </c>
+      <c r="D80"/>
+      <c r="E80" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
+        <v>84</v>
+      </c>
+      <c r="C81" t="s">
+        <v>7</v>
+      </c>
+      <c r="D81"/>
+      <c r="E81" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
+        <v>85</v>
+      </c>
+      <c r="C82" t="s">
+        <v>7</v>
+      </c>
+      <c r="D82"/>
+      <c r="E82" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
+        <v>86</v>
+      </c>
+      <c r="C83" t="s">
+        <v>7</v>
+      </c>
+      <c r="D83"/>
+      <c r="E83" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84" t="s">
+        <v>87</v>
+      </c>
+      <c r="C84" t="s">
+        <v>7</v>
+      </c>
+      <c r="D84"/>
+      <c r="E84" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
+        <v>88</v>
+      </c>
+      <c r="C85" t="s">
+        <v>7</v>
+      </c>
+      <c r="D85"/>
+      <c r="E85" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
+        <v>89</v>
+      </c>
+      <c r="C86" t="s">
+        <v>7</v>
+      </c>
+      <c r="D86"/>
+      <c r="E86" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87" t="s">
+        <v>90</v>
+      </c>
+      <c r="C87" t="s">
+        <v>7</v>
+      </c>
+      <c r="D87"/>
+      <c r="E87" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88" t="s">
+        <v>91</v>
+      </c>
+      <c r="C88" t="s">
+        <v>7</v>
+      </c>
+      <c r="D88"/>
+      <c r="E88" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89" t="s">
+        <v>92</v>
+      </c>
+      <c r="C89" t="s">
+        <v>7</v>
+      </c>
+      <c r="D89"/>
+      <c r="E89" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90" t="s">
+        <v>93</v>
+      </c>
+      <c r="C90" t="s">
+        <v>7</v>
+      </c>
+      <c r="D90"/>
+      <c r="E90" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91" t="s">
+        <v>94</v>
+      </c>
+      <c r="C91" t="s">
+        <v>7</v>
+      </c>
+      <c r="D91"/>
+      <c r="E91" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92" t="s">
+        <v>95</v>
+      </c>
+      <c r="C92" t="s">
+        <v>7</v>
+      </c>
+      <c r="D92"/>
+      <c r="E92" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93" t="s">
+        <v>96</v>
+      </c>
+      <c r="C93" t="s">
+        <v>7</v>
+      </c>
+      <c r="D93"/>
+      <c r="E93" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94" t="s">
+        <v>97</v>
+      </c>
+      <c r="C94" t="s">
+        <v>7</v>
+      </c>
+      <c r="D94"/>
+      <c r="E94" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95" t="s">
+        <v>98</v>
+      </c>
+      <c r="C95" t="s">
+        <v>7</v>
+      </c>
+      <c r="D95"/>
+      <c r="E95" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96" t="s">
+        <v>99</v>
+      </c>
+      <c r="C96" t="s">
+        <v>7</v>
+      </c>
+      <c r="D96"/>
+      <c r="E96" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97" t="s">
+        <v>100</v>
+      </c>
+      <c r="C97" t="s">
+        <v>7</v>
+      </c>
+      <c r="D97"/>
+      <c r="E97" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98" t="s">
+        <v>101</v>
+      </c>
+      <c r="C98" t="s">
+        <v>7</v>
+      </c>
+      <c r="D98"/>
+      <c r="E98" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99" t="s">
+        <v>102</v>
+      </c>
+      <c r="C99" t="s">
+        <v>7</v>
+      </c>
+      <c r="D99"/>
+      <c r="E99" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100" t="s">
+        <v>103</v>
+      </c>
+      <c r="C100" t="s">
+        <v>7</v>
+      </c>
+      <c r="D100"/>
+      <c r="E100" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101" t="s">
+        <v>104</v>
+      </c>
+      <c r="C101" t="s">
+        <v>7</v>
+      </c>
+      <c r="D101"/>
+      <c r="E101" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9">
+      <c r="A102">
+        <v>101</v>
+      </c>
+      <c r="B102" t="s">
+        <v>105</v>
+      </c>
+      <c r="C102" t="s">
+        <v>7</v>
+      </c>
+      <c r="D102"/>
+      <c r="E102" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9">
+      <c r="A103">
+        <v>102</v>
+      </c>
+      <c r="B103" t="s">
+        <v>106</v>
+      </c>
+      <c r="C103" t="s">
+        <v>7</v>
+      </c>
+      <c r="D103"/>
+      <c r="E103" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9">
+      <c r="A104">
+        <v>103</v>
+      </c>
+      <c r="B104" t="s">
+        <v>107</v>
+      </c>
+      <c r="C104" t="s">
+        <v>7</v>
+      </c>
+      <c r="D104"/>
+      <c r="E104" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9">
+      <c r="A105">
+        <v>104</v>
+      </c>
+      <c r="B105" t="s">
+        <v>13</v>
+      </c>
+      <c r="C105" t="s">
+        <v>7</v>
+      </c>
+      <c r="D105"/>
+      <c r="E105" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9">
+      <c r="A106">
+        <v>105</v>
+      </c>
+      <c r="B106" t="s">
+        <v>108</v>
+      </c>
+      <c r="C106" t="s">
+        <v>7</v>
+      </c>
+      <c r="D106"/>
+      <c r="E106" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9">
+      <c r="A107">
+        <v>106</v>
+      </c>
+      <c r="B107" t="s">
+        <v>105</v>
+      </c>
+      <c r="C107" t="s">
+        <v>7</v>
+      </c>
+      <c r="D107"/>
+      <c r="E107" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9">
+      <c r="A108">
+        <v>107</v>
+      </c>
+      <c r="B108" t="s">
+        <v>109</v>
+      </c>
+      <c r="C108" t="s">
+        <v>7</v>
+      </c>
+      <c r="D108"/>
+      <c r="E108" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9">
+      <c r="A109">
+        <v>108</v>
+      </c>
+      <c r="B109" t="s">
+        <v>110</v>
+      </c>
+      <c r="C109" t="s">
+        <v>7</v>
+      </c>
+      <c r="D109"/>
+      <c r="E109" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9">
+      <c r="A110">
+        <v>109</v>
+      </c>
+      <c r="B110" t="s">
+        <v>111</v>
+      </c>
+      <c r="C110" t="s">
+        <v>7</v>
+      </c>
+      <c r="D110"/>
+      <c r="E110" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9">
+      <c r="A111">
+        <v>110</v>
+      </c>
+      <c r="B111" t="s">
+        <v>112</v>
+      </c>
+      <c r="C111" t="s">
+        <v>7</v>
+      </c>
+      <c r="D111"/>
+      <c r="E111" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9">
+      <c r="A112">
+        <v>111</v>
+      </c>
+      <c r="B112" t="s">
+        <v>113</v>
+      </c>
+      <c r="C112" t="s">
+        <v>7</v>
+      </c>
+      <c r="D112"/>
+      <c r="E112" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9">
+      <c r="A113">
+        <v>112</v>
+      </c>
+      <c r="B113" t="s">
+        <v>114</v>
+      </c>
+      <c r="C113" t="s">
+        <v>7</v>
+      </c>
+      <c r="D113"/>
+      <c r="E113" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9">
+      <c r="A114">
+        <v>113</v>
+      </c>
+      <c r="B114" t="s">
+        <v>115</v>
+      </c>
+      <c r="C114" t="s">
+        <v>7</v>
+      </c>
+      <c r="D114"/>
+      <c r="E114" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9">
+      <c r="A115">
+        <v>114</v>
+      </c>
+      <c r="B115" t="s">
+        <v>116</v>
+      </c>
+      <c r="C115" t="s">
+        <v>7</v>
+      </c>
+      <c r="D115"/>
+      <c r="E115" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9">
+      <c r="A116">
+        <v>115</v>
+      </c>
+      <c r="B116" t="s">
+        <v>117</v>
+      </c>
+      <c r="C116" t="s">
+        <v>7</v>
+      </c>
+      <c r="D116"/>
+      <c r="E116" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9">
+      <c r="A117">
+        <v>116</v>
+      </c>
+      <c r="B117" t="s">
+        <v>118</v>
+      </c>
+      <c r="C117" t="s">
+        <v>7</v>
+      </c>
+      <c r="D117"/>
+      <c r="E117" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9">
+      <c r="A118">
+        <v>117</v>
+      </c>
+      <c r="B118" t="s">
+        <v>119</v>
+      </c>
+      <c r="C118" t="s">
+        <v>7</v>
+      </c>
+      <c r="D118"/>
+      <c r="E118" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9">
+      <c r="A119">
+        <v>118</v>
+      </c>
+      <c r="B119" t="s">
+        <v>120</v>
+      </c>
+      <c r="C119" t="s">
+        <v>7</v>
+      </c>
+      <c r="D119"/>
+      <c r="E119" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9">
+      <c r="A120">
+        <v>119</v>
+      </c>
+      <c r="B120" t="s">
+        <v>121</v>
+      </c>
+      <c r="C120" t="s">
+        <v>7</v>
+      </c>
+      <c r="D120"/>
+      <c r="E120" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9">
+      <c r="A121">
+        <v>120</v>
+      </c>
+      <c r="B121" t="s">
+        <v>122</v>
+      </c>
+      <c r="C121" t="s">
+        <v>7</v>
+      </c>
+      <c r="D121"/>
+      <c r="E121" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9">
+      <c r="A122">
+        <v>121</v>
+      </c>
+      <c r="B122" t="s">
+        <v>123</v>
+      </c>
+      <c r="C122" t="s">
+        <v>7</v>
+      </c>
+      <c r="D122"/>
+      <c r="E122" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9">
+      <c r="A123">
+        <v>122</v>
+      </c>
+      <c r="B123" t="s">
+        <v>124</v>
+      </c>
+      <c r="C123" t="s">
+        <v>7</v>
+      </c>
+      <c r="D123"/>
+      <c r="E123" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9">
+      <c r="A124">
+        <v>123</v>
+      </c>
+      <c r="B124" t="s">
+        <v>125</v>
+      </c>
+      <c r="C124" t="s">
+        <v>7</v>
+      </c>
+      <c r="D124"/>
+      <c r="E124" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9">
+      <c r="A125">
+        <v>124</v>
+      </c>
+      <c r="B125" t="s">
+        <v>126</v>
+      </c>
+      <c r="C125" t="s">
+        <v>7</v>
+      </c>
+      <c r="D125"/>
+      <c r="E125" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9">
+      <c r="A126">
+        <v>125</v>
+      </c>
+      <c r="B126" t="s">
+        <v>127</v>
+      </c>
+      <c r="C126" t="s">
+        <v>7</v>
+      </c>
+      <c r="D126"/>
+      <c r="E126" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9">
+      <c r="A127">
+        <v>126</v>
+      </c>
+      <c r="B127" t="s">
+        <v>128</v>
+      </c>
+      <c r="C127" t="s">
+        <v>7</v>
+      </c>
+      <c r="D127"/>
+      <c r="E127" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9">
+      <c r="A128">
+        <v>127</v>
+      </c>
+      <c r="B128" t="s">
+        <v>129</v>
+      </c>
+      <c r="C128" t="s">
+        <v>7</v>
+      </c>
+      <c r="D128"/>
+      <c r="E128" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9">
+      <c r="A129">
+        <v>128</v>
+      </c>
+      <c r="B129" t="s">
+        <v>130</v>
+      </c>
+      <c r="C129" t="s">
+        <v>7</v>
+      </c>
+      <c r="D129"/>
+      <c r="E129" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9">
+      <c r="A130">
+        <v>129</v>
+      </c>
+      <c r="B130" t="s">
+        <v>131</v>
+      </c>
+      <c r="C130" t="s">
+        <v>7</v>
+      </c>
+      <c r="D130"/>
+      <c r="E130" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9">
+      <c r="A131">
+        <v>130</v>
+      </c>
+      <c r="B131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C131" t="s">
+        <v>7</v>
+      </c>
+      <c r="D131"/>
+      <c r="E131" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9">
+      <c r="A132">
+        <v>131</v>
+      </c>
+      <c r="B132" t="s">
+        <v>133</v>
+      </c>
+      <c r="C132" t="s">
+        <v>7</v>
+      </c>
+      <c r="D132"/>
+      <c r="E132" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9">
+      <c r="A133">
+        <v>132</v>
+      </c>
+      <c r="B133" t="s">
+        <v>134</v>
+      </c>
+      <c r="C133" t="s">
+        <v>7</v>
+      </c>
+      <c r="D133"/>
+      <c r="E133" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9">
+      <c r="A134">
+        <v>133</v>
+      </c>
+      <c r="B134" t="s">
+        <v>135</v>
+      </c>
+      <c r="C134" t="s">
+        <v>7</v>
+      </c>
+      <c r="D134"/>
+      <c r="E134" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9">
+      <c r="A135">
+        <v>134</v>
+      </c>
+      <c r="B135" t="s">
+        <v>136</v>
+      </c>
+      <c r="C135" t="s">
+        <v>7</v>
+      </c>
+      <c r="D135"/>
+      <c r="E135" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9">
+      <c r="A136">
+        <v>139</v>
+      </c>
+      <c r="B136" t="s">
+        <v>137</v>
+      </c>
+      <c r="C136" t="s">
+        <v>7</v>
+      </c>
+      <c r="D136"/>
+      <c r="E136" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9">
+      <c r="A137">
+        <v>140</v>
+      </c>
+      <c r="B137" t="s">
+        <v>138</v>
+      </c>
+      <c r="C137" t="s">
+        <v>7</v>
+      </c>
+      <c r="D137"/>
+      <c r="E137" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9">
+      <c r="A138">
+        <v>141</v>
+      </c>
+      <c r="B138" t="s">
+        <v>139</v>
+      </c>
+      <c r="C138" t="s">
+        <v>7</v>
+      </c>
+      <c r="D138"/>
+      <c r="E138" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9">
+      <c r="A139">
+        <v>142</v>
+      </c>
+      <c r="B139" t="s">
+        <v>140</v>
+      </c>
+      <c r="C139" t="s">
+        <v>7</v>
+      </c>
+      <c r="D139"/>
+      <c r="E139" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9">
+      <c r="A140">
+        <v>143</v>
+      </c>
+      <c r="B140" t="s">
+        <v>141</v>
+      </c>
+      <c r="C140" t="s">
+        <v>7</v>
+      </c>
+      <c r="D140"/>
+      <c r="E140" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9">
+      <c r="A141">
+        <v>144</v>
+      </c>
+      <c r="B141" t="s">
+        <v>27</v>
+      </c>
+      <c r="C141" t="s">
+        <v>7</v>
+      </c>
+      <c r="D141"/>
+      <c r="E141" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9">
+      <c r="A142">
+        <v>145</v>
+      </c>
+      <c r="B142" t="s">
+        <v>142</v>
+      </c>
+      <c r="C142" t="s">
+        <v>7</v>
+      </c>
+      <c r="D142"/>
+      <c r="E142" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9">
+      <c r="A143">
+        <v>146</v>
+      </c>
+      <c r="B143" t="s">
+        <v>143</v>
+      </c>
+      <c r="C143" t="s">
+        <v>7</v>
+      </c>
+      <c r="D143"/>
+      <c r="E143" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>